<commit_message>
crawler update again 3
</commit_message>
<xml_diff>
--- a/Document/4_수정중/크롤링 결과(2차).xlsx
+++ b/Document/4_수정중/크롤링 결과(2차).xlsx
@@ -8,9 +8,9 @@
       <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\user\git\ChemicalManagementApplication\Document\4_수정중\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B4FDADF3-135E-4DEE-BCD7-B277519FECC5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{B9A3C793-FC3E-4A88-AEDD-10452D3BDFB5}" xr6:coauthVersionLast="41" xr6:coauthVersionMax="41" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-108" yWindow="492" windowWidth="23256" windowHeight="12576" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="1464" yWindow="2064" windowWidth="17280" windowHeight="8964" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet" sheetId="1" r:id="rId1"/>
@@ -743,8 +743,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:R16"/>
   <sheetViews>
-    <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A15" sqref="A15"/>
+    <sheetView tabSelected="1" topLeftCell="A3" workbookViewId="0">
+      <selection activeCell="C11" sqref="C11"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr defaultRowHeight="17.399999999999999"/>
@@ -997,7 +997,7 @@
         <v>-218.79</v>
       </c>
       <c r="H5" s="7">
-        <v>182.96199999999999</v>
+        <v>-182.96199999999999</v>
       </c>
       <c r="I5">
         <v>0</v>

</xml_diff>